<commit_message>
fixed code until point (g)
</commit_message>
<xml_diff>
--- a/Alessia/PS3/Table1.xlsx
+++ b/Alessia/PS3/Table1.xlsx
@@ -13,10 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="24">
-  <si>
-    <t>Variable</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="14" uniqueCount="14">
   <si>
     <t>Label</t>
   </si>
@@ -24,55 +21,28 @@
     <t>Share Men aged 15-20 with High School Education</t>
   </si>
   <si>
-    <t>hischshr1520m</t>
-  </si>
-  <si>
     <t>Islamic Mayor in 1989</t>
   </si>
   <si>
-    <t>i89</t>
-  </si>
-  <si>
     <t>Islamic vote share 1994</t>
   </si>
   <si>
-    <t>vshr_islam1994</t>
-  </si>
-  <si>
     <t>Number of parties receiving votes 1994</t>
   </si>
   <si>
-    <t>partycount</t>
-  </si>
-  <si>
     <t>Log Population in 1994</t>
   </si>
   <si>
-    <t>lpop1994</t>
-  </si>
-  <si>
     <t>District center</t>
   </si>
   <si>
-    <t>merkezi</t>
-  </si>
-  <si>
     <t>Province center</t>
   </si>
   <si>
-    <t>merkezp</t>
-  </si>
-  <si>
     <t>Sub-metro center</t>
   </si>
   <si>
-    <t>subbuyuk</t>
-  </si>
-  <si>
     <t>Metro center</t>
-  </si>
-  <si>
-    <t>buyuk</t>
   </si>
   <si>
     <t>MSE-Optimal Bandwidth</t>
@@ -138,28 +108,22 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>12.055</v>
@@ -176,10 +140,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>11.783</v>
@@ -196,10 +157,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>13.94</v>
@@ -216,10 +174,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>12.166</v>
@@ -236,10 +191,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>13.32</v>
@@ -256,10 +208,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>13.033</v>
@@ -276,10 +225,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>11.557</v>
@@ -296,10 +242,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>10.36</v>
@@ -316,10 +259,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>13.622</v>

</xml_diff>